<commit_message>
Initial files from SESYNC 2106 course
</commit_message>
<xml_diff>
--- a/Labs/HemlockLightExample/HemlockLightLikelihoodAnswers.xlsx
+++ b/Labs/HemlockLightExample/HemlockLightLikelihoodAnswers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="NORMAL LIKELIHOOD" sheetId="8" r:id="rId1"/>
@@ -51,8 +51,10 @@
     <definedName name="solver_mda" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">5000</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">5000</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mod" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_mod" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_mtr" localSheetId="0" hidden="1">0</definedName>
@@ -67,6 +69,7 @@
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'NORMAL LIKELIHOOD'!$K$2</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'NORMAL LIKELIHOOD PLUS PRIOR'!#REF!</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
@@ -78,6 +81,7 @@
     <definedName name="solver_rep" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rtr" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rtr" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
@@ -247,8 +251,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -298,19 +312,29 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1193,235 +1217,235 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="77"/>
                 <c:pt idx="0">
-                  <c:v>30.39382205418087</c:v>
+                  <c:v>31.18794109833727</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.39382205418087</c:v>
+                  <c:v>31.18794109833727</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.39382205418087</c:v>
+                  <c:v>31.18794109833727</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.66304615220135</c:v>
+                  <c:v>17.64552412510712</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.371282600698803</c:v>
+                  <c:v>9.266857043595267</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.371282600698803</c:v>
+                  <c:v>9.266857043595267</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.39846366031675</c:v>
+                  <c:v>15.32387252332576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.39846366031675</c:v>
+                  <c:v>15.32387252332576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.40539980015102</c:v>
+                  <c:v>31.2006505484418</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.40539980015102</c:v>
+                  <c:v>31.2006505484418</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.40539980015102</c:v>
+                  <c:v>31.2006505484418</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.427197026268258</c:v>
+                  <c:v>8.333819149397903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.602556094792659</c:v>
+                  <c:v>2.668686761252268</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.602556094792659</c:v>
+                  <c:v>2.668686761252268</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.642527572534978</c:v>
+                  <c:v>8.546261086100806</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25.57021470455664</c:v>
+                  <c:v>25.9562748266046</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26.68614782447437</c:v>
+                  <c:v>27.15546136018255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.50784318563118</c:v>
+                  <c:v>26.9634082289349</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.09396249796202</c:v>
+                  <c:v>26.51826952957539</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26.0806702775374</c:v>
+                  <c:v>26.50398857592698</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26.60365131283237</c:v>
+                  <c:v>27.06658266124903</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.95653194944796</c:v>
+                  <c:v>28.5287417527813</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28.28414924399915</c:v>
+                  <c:v>28.88430660383549</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28.69046174738873</c:v>
+                  <c:v>29.32608798844402</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.22713268941388</c:v>
+                  <c:v>17.19664136399585</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>27.55840744108952</c:v>
+                  <c:v>28.09743589680479</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.2834597147883</c:v>
+                  <c:v>10.17235505037912</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.06234631520798</c:v>
+                  <c:v>20.13333176317763</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>23.31064358905971</c:v>
+                  <c:v>23.54832595489016</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.27130649714394</c:v>
+                  <c:v>20.35138240899738</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>19.94875204881352</c:v>
+                  <c:v>20.01488920552583</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>28.3028842252242</c:v>
+                  <c:v>28.90465735109939</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>30.36469904955903</c:v>
+                  <c:v>31.15597463459795</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30.36469904955903</c:v>
+                  <c:v>31.15597463459795</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>30.36469904955903</c:v>
+                  <c:v>31.15597463459795</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.263152231859194</c:v>
+                  <c:v>1.387774231144407</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.295787377223264</c:v>
+                  <c:v>3.334809248189255</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>23.18600883452187</c:v>
+                  <c:v>23.416286942539</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>19.99575537869768</c:v>
+                  <c:v>20.06389069740403</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>22.97046117642365</c:v>
+                  <c:v>23.18812535669787</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>24.20703136583611</c:v>
+                  <c:v>24.50036047501598</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>22.97046117642365</c:v>
+                  <c:v>23.18812535669787</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>26.51792680243313</c:v>
+                  <c:v>26.97426482284691</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>26.0806702775374</c:v>
+                  <c:v>26.50398857592698</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>20.20110345848713</c:v>
+                  <c:v>20.27810044773791</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>23.19006472371211</c:v>
+                  <c:v>23.42058250630162</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>14.92772946700781</c:v>
+                  <c:v>14.8444623598216</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>14.51086769553724</c:v>
+                  <c:v>14.4208263379733</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>18.55454641790416</c:v>
+                  <c:v>18.56651622702044</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>26.61742063657415</c:v>
+                  <c:v>27.08141468995448</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>18.80077395310177</c:v>
+                  <c:v>18.82159452713933</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>12.6352898747724</c:v>
+                  <c:v>12.52526007827672</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>11.92077154549511</c:v>
+                  <c:v>11.80760992332072</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>24.0975858073591</c:v>
+                  <c:v>24.38389482403989</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>22.67919444970194</c:v>
+                  <c:v>22.88019802298183</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>27.80380828008811</c:v>
+                  <c:v>28.36318829323787</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>23.23527814753358</c:v>
+                  <c:v>23.46847353831289</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>12.17802790830518</c:v>
+                  <c:v>12.06571051985712</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>12.17802790830518</c:v>
+                  <c:v>12.06571051985712</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>19.4193679191169</c:v>
+                  <c:v>19.4637767666045</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>15.59324618841245</c:v>
+                  <c:v>15.52256426902631</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>17.33614512655544</c:v>
+                  <c:v>17.30880802875247</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30.38220358399848</c:v>
+                  <c:v>31.17518768521671</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>30.38220358399848</c:v>
+                  <c:v>31.17518768521671</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>30.38220358399848</c:v>
+                  <c:v>31.17518768521671</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.37696138718957</c:v>
+                  <c:v>4.378043801685221</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.37696138718957</c:v>
+                  <c:v>4.378043801685221</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.87463482017162</c:v>
+                  <c:v>5.831967045505373</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.87463482017162</c:v>
+                  <c:v>5.831967045505373</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.87463482017162</c:v>
+                  <c:v>5.831967045505373</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>23.72595145875037</c:v>
+                  <c:v>23.98889226125055</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>24.20268050066658</c:v>
+                  <c:v>24.49572933363256</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>23.54463064250031</c:v>
+                  <c:v>23.79643280552122</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>29.1543572648301</c:v>
+                  <c:v>29.83157641192689</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>29.34150511533951</c:v>
+                  <c:v>30.03583603001242</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>29.39252327108659</c:v>
+                  <c:v>30.09155217965956</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>29.57462133012711</c:v>
+                  <c:v>30.29053471440159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1436,11 +1460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2096964616"/>
-        <c:axId val="2096972568"/>
+        <c:axId val="2101842616"/>
+        <c:axId val="2101852008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2096964616"/>
+        <c:axId val="2101842616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -1487,12 +1511,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096972568"/>
+        <c:crossAx val="2101852008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2096972568"/>
+        <c:axId val="2101852008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096964616"/>
+        <c:crossAx val="2101842616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
@@ -2623,11 +2647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097011064"/>
-        <c:axId val="2097019256"/>
+        <c:axId val="2101925576"/>
+        <c:axId val="2101933768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097011064"/>
+        <c:axId val="2101925576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2674,12 +2698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2097019256"/>
+        <c:crossAx val="2101933768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097019256"/>
+        <c:axId val="2101933768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2725,7 +2749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2097011064"/>
+        <c:crossAx val="2101925576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
@@ -2771,7 +2795,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -3158,9 +3182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6:I6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>
@@ -3170,8 +3194,8 @@
     <col min="4" max="4" width="15.83203125" style="4" customWidth="1"/>
     <col min="5" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="3.83203125" style="1" customWidth="1"/>
-    <col min="8" max="27" width="22" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="25" width="22" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1">
@@ -3215,32 +3239,32 @@
       </c>
       <c r="C2" s="10">
         <f t="shared" ref="C2:C33" si="0">alpha*(A2-c_)/(alpha/gamma+(A2-c_))</f>
-        <v>30.393822054180866</v>
+        <v>31.187941098337269</v>
       </c>
       <c r="D2" s="4">
         <f>(C2-B2)^2</f>
-        <v>149.50332887041671</v>
+        <v>169.55358782487772</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ref="E2:E33" si="1">NORMDIST(B2,C2,$I$5,FALSE)</f>
-        <v>1.3339455822494989E-2</v>
+        <v>1.1377871214859574E-2</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F65" si="2">LN(E2)</f>
-        <v>-4.3170290322431306</v>
+        <v>-4.4760849315031521</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="6">
-        <v>37</v>
+        <v>38.561814977884261</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="6">
         <f>SUM(F2:F78)</f>
-        <v>-262.03972641960883</v>
+        <v>-261.94334572940329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1">
@@ -3252,25 +3276,25 @@
       </c>
       <c r="C3" s="10">
         <f t="shared" si="0"/>
-        <v>30.393822054180866</v>
+        <v>31.187941098337269</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D66" si="3">(C3-B3)^2</f>
-        <v>19.305672243806168</v>
+        <v>26.914732839816914</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" si="1"/>
-        <v>4.5714913070997211E-2</v>
+        <v>4.2241026624860081E-2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0853307089097797</v>
+        <v>-3.164363335313666</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>1.8191090298589145</v>
+        <v>1.7408825565402852</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22" customHeight="1">
@@ -3282,25 +3306,25 @@
       </c>
       <c r="C4" s="10">
         <f t="shared" si="0"/>
-        <v>30.393822054180866</v>
+        <v>31.187941098337269</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="3"/>
-        <v>22.345998057704207</v>
+        <v>30.48447134981917</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="1"/>
-        <v>4.4418783089929706E-2</v>
+        <v>4.0876865233452145E-2</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1140928564352515</v>
+        <v>-3.1971910181831737</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="6">
-        <v>4.9210768872418882</v>
+        <v>4.8130732496314836</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="22" customHeight="1">
@@ -3312,25 +3336,25 @@
       </c>
       <c r="C5" s="10">
         <f t="shared" si="0"/>
-        <v>17.66304615220135</v>
+        <v>17.645524125107119</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="3"/>
-        <v>132.16674127542262</v>
+        <v>131.76416855119393</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="1"/>
-        <v>1.5716862164471004E-2</v>
+        <v>1.6105901181173596E-2</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="2"/>
-        <v>-4.153021119763455</v>
+        <v>-4.1285695411563781</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="6">
-        <v>7.27</v>
+        <v>7.373659683205525</v>
       </c>
       <c r="K5" s="4"/>
     </row>
@@ -3343,26 +3367,25 @@
       </c>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
-        <v>9.3712826006988035</v>
+        <v>9.2668570435952677</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="3"/>
-        <v>0.39528556818406019</v>
+        <v>0.53749859452587112</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="1"/>
-        <v>5.4670320003486546E-2</v>
+        <v>5.3836932294271653E-2</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9064343127269576</v>
+        <v>-2.9217955734585885</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="6">
-        <f>SQRT(AVERAGE(D2:D78))</f>
-        <v>7.273041897681864</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="22" customHeight="1">
@@ -3374,19 +3397,19 @@
       </c>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
-        <v>9.3712826006988035</v>
+        <v>9.2668570435952677</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="3"/>
-        <v>3.2234039443314155</v>
+        <v>3.6092766039148168</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="1"/>
-        <v>5.3227029867195061E-2</v>
+        <v>5.2337405130056643E-2</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9331889314531523</v>
+        <v>-2.9500439602956638</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="22" customHeight="1">
@@ -3398,19 +3421,19 @@
       </c>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
-        <v>15.398463660316748</v>
+        <v>15.323872523325765</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="3"/>
-        <v>65.046327191227661</v>
+        <v>63.848716546804951</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="1"/>
-        <v>2.9657290029086899E-2</v>
+        <v>3.0076472658604653E-2</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="2"/>
-        <v>-3.518047314312903</v>
+        <v>-3.5040120521155562</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="22" customHeight="1">
@@ -3422,19 +3445,19 @@
       </c>
       <c r="C9" s="10">
         <f t="shared" si="0"/>
-        <v>15.398463660316748</v>
+        <v>15.323872523325765</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="3"/>
-        <v>7.1932852615152088E-2</v>
+        <v>0.1175078247088456</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="1"/>
-        <v>5.4837811873409262E-2</v>
+        <v>5.404526757831344E-2</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9033753252771781</v>
+        <v>-2.9179332950981314</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="22" customHeight="1">
@@ -3446,19 +3469,19 @@
       </c>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
-        <v>30.405399800151024</v>
+        <v>31.2006505484418</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="3"/>
-        <v>189.37246577146217</v>
+        <v>168.1175739780679</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="1"/>
-        <v>9.1481848900889975E-3</v>
+        <v>1.152912080624369E-2</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="2"/>
-        <v>-4.6941997920410365</v>
+        <v>-4.4628792003194233</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="22" customHeight="1">
@@ -3470,19 +3493,19 @@
       </c>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
-        <v>30.405399800151024</v>
+        <v>31.2006505484418</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="3"/>
-        <v>85.771063972821096</v>
+        <v>71.673428914043797</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="1"/>
-        <v>2.4377179284788976E-2</v>
+        <v>2.7988294419651984E-2</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="2"/>
-        <v>-3.7141078595393089</v>
+        <v>-3.5759689126578902</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="22" customHeight="1">
@@ -3494,19 +3517,19 @@
       </c>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
-        <v>30.405399800151024</v>
+        <v>31.2006505484418</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="3"/>
-        <v>0.16434899796248997</v>
+        <v>1.4415617394735951</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="1"/>
-        <v>5.4789889389833597E-2</v>
+        <v>5.3391195161895215E-2</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9042496022359385</v>
+        <v>-2.9301094312196532</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="22" customHeight="1">
@@ -3518,19 +3541,19 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
-        <v>8.4271970262682583</v>
+        <v>8.3338191493979039</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="3"/>
-        <v>12.915856243395877</v>
+        <v>12.253400948469263</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>4.8563568368102585E-2</v>
+        <v>4.8338051258624226E-2</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0248816512382959</v>
+        <v>-3.0295362177460401</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="22" customHeight="1">
@@ -3542,19 +3565,19 @@
       </c>
       <c r="C14" s="10">
         <f t="shared" si="0"/>
-        <v>2.6025560947926594</v>
+        <v>2.668686761252268</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="3"/>
-        <v>2.4464418810480435</v>
+        <v>2.2439437970253397</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="1"/>
-        <v>5.3619702188128684E-2</v>
+        <v>5.2998682764854019E-2</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9258387003089443</v>
+        <v>-2.9374882192321889</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="22" customHeight="1">
@@ -3566,19 +3589,19 @@
       </c>
       <c r="C15" s="10">
         <f t="shared" si="0"/>
-        <v>2.6025560947926594</v>
+        <v>2.668686761252268</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="3"/>
-        <v>7.4571443265318127</v>
+        <v>7.1003413541033567</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="1"/>
-        <v>5.1137303313915999E-2</v>
+        <v>5.0683840288662976E-2</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9732410419541879</v>
+        <v>-2.9821481511698669</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1">
@@ -3590,19 +3613,19 @@
       </c>
       <c r="C16" s="10">
         <f t="shared" si="0"/>
-        <v>8.6425275725349788</v>
+        <v>8.5462610861008059</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="3"/>
-        <v>15.807469942811972</v>
+        <v>15.051252859304492</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="1"/>
-        <v>4.7253103265727237E-2</v>
+        <v>4.7110208899965499E-2</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0522369496175346</v>
+        <v>-3.0552655519780552</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="22" customHeight="1">
@@ -3614,19 +3637,19 @@
       </c>
       <c r="C17" s="10">
         <f t="shared" si="0"/>
-        <v>25.570214704556641</v>
+        <v>25.956274826604595</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="3"/>
-        <v>6.7415627915451761</v>
+        <v>4.8858320866131377</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>5.1484654631212448E-2</v>
+        <v>5.1726591054690838E-2</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9664714840398005</v>
+        <v>-2.961783295945581</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="22" customHeight="1">
@@ -3638,19 +3661,19 @@
       </c>
       <c r="C18" s="10">
         <f t="shared" si="0"/>
-        <v>26.686147824474375</v>
+        <v>27.155461360182553</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="3"/>
-        <v>16.156228777970931</v>
+        <v>20.149277800536083</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="1"/>
-        <v>4.7097456359777752E-2</v>
+        <v>4.4952562395943273E-2</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0555362845183529</v>
+        <v>-3.1021475142177724</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="22" customHeight="1">
@@ -3662,19 +3685,19 @@
       </c>
       <c r="C19" s="10">
         <f t="shared" si="0"/>
-        <v>26.507843185631181</v>
+        <v>26.963408228934899</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="3"/>
-        <v>96.540256642591416</v>
+        <v>87.795496462035388</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="1"/>
-        <v>2.2015978828823675E-2</v>
+        <v>2.413169624484655E-2</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="2"/>
-        <v>-3.8159867788584978</v>
+        <v>-3.7242291057177765</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="22" customHeight="1">
@@ -3686,19 +3709,19 @@
       </c>
       <c r="C20" s="10">
         <f t="shared" si="0"/>
-        <v>26.093962497962018</v>
+        <v>26.518269529575392</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="3"/>
-        <v>126.32345677499455</v>
+        <v>116.96560507935448</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" si="1"/>
-        <v>1.6610132642600917E-2</v>
+        <v>1.8453883776709524E-2</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="2"/>
-        <v>-4.0977423696813586</v>
+        <v>-3.992480427845523</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="22" customHeight="1">
@@ -3710,19 +3733,19 @@
       </c>
       <c r="C21" s="10">
         <f t="shared" si="0"/>
-        <v>26.080670277537404</v>
+        <v>26.503988575926982</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="3"/>
-        <v>85.611773624090247</v>
+        <v>77.957328845138434</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="1"/>
-        <v>2.4413941473665376E-2</v>
+        <v>2.6416768410487498E-2</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="2"/>
-        <v>-3.7126009379822058</v>
+        <v>-3.6337563033991698</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="22" customHeight="1">
@@ -3734,19 +3757,19 @@
       </c>
       <c r="C22" s="10">
         <f t="shared" si="0"/>
-        <v>26.603651312832373</v>
+        <v>27.066582661249033</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="3"/>
-        <v>113.34474036875586</v>
+        <v>103.70198869517382</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="1"/>
-        <v>1.8780036299996188E-2</v>
+        <v>2.0847800123103149E-2</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="2"/>
-        <v>-3.9749608722967431</v>
+        <v>-3.8705068459871672</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="22" customHeight="1">
@@ -3758,19 +3781,19 @@
       </c>
       <c r="C23" s="10">
         <f t="shared" si="0"/>
-        <v>27.956531949447957</v>
+        <v>28.528741752781301</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="3"/>
-        <v>34.536794505636685</v>
+        <v>28.138691836463163</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" si="1"/>
-        <v>3.9580430641328886E-2</v>
+        <v>4.1768242030023627E-2</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="2"/>
-        <v>-3.2294204585907855</v>
+        <v>-3.1756189882626429</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="22" customHeight="1">
@@ -3782,19 +3805,19 @@
       </c>
       <c r="C24" s="10">
         <f t="shared" si="0"/>
-        <v>28.284149243999153</v>
+        <v>28.884306603835491</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="3"/>
-        <v>13.807546840872069</v>
+        <v>9.7075453389031345</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="1"/>
-        <v>4.8155629127363798E-2</v>
+        <v>4.9483090815866569E-2</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0333172394224466</v>
+        <v>-3.0061242674454167</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22" customHeight="1">
@@ -3806,19 +3829,19 @@
       </c>
       <c r="C25" s="10">
         <f t="shared" si="0"/>
-        <v>28.690461747388728</v>
+        <v>29.326087988444019</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="3"/>
-        <v>29.988820317924262</v>
+        <v>23.431201940064032</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>4.132053746125005E-2</v>
+        <v>4.3616121992564594E-2</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1863956275246337</v>
+        <v>-3.1323284265037361</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="22" customHeight="1">
@@ -3830,19 +3853,19 @@
       </c>
       <c r="C26" s="10">
         <f t="shared" si="0"/>
-        <v>17.227132689413882</v>
+        <v>17.196641363995848</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="3"/>
-        <v>22.345783463325319</v>
+        <v>22.05844010199678</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="1"/>
-        <v>4.4418873265027421E-2</v>
+        <v>4.417022465224018E-2</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1140908263254663</v>
+        <v>-3.119704367304676</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="22" customHeight="1">
@@ -3854,19 +3877,19 @@
       </c>
       <c r="C27" s="10">
         <f t="shared" si="0"/>
-        <v>27.558407441089525</v>
+        <v>28.097435896804789</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="3"/>
-        <v>1.9369423831910446</v>
+        <v>3.7278698200480314</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="1"/>
-        <v>5.3878771758863214E-2</v>
+        <v>5.2280357309133232E-2</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="2"/>
-        <v>-2.921018723563515</v>
+        <v>-2.9511345557212914</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="22" customHeight="1">
@@ -3878,19 +3901,19 @@
       </c>
       <c r="C28" s="10">
         <f t="shared" si="0"/>
-        <v>10.283459714788293</v>
+        <v>10.172355050379123</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="3"/>
-        <v>1.4799702655429812</v>
+        <v>1.7626411122538219</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="1"/>
-        <v>5.4112196910481483E-2</v>
+        <v>5.3233780614454787E-2</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9166956673296278</v>
+        <v>-2.9330621101892853</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="22" customHeight="1">
@@ -3902,19 +3925,19 @@
       </c>
       <c r="C29" s="10">
         <f t="shared" si="0"/>
-        <v>20.062346315207982</v>
+        <v>20.133331763177633</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="3"/>
-        <v>157.81254494321956</v>
+        <v>159.60107143851289</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>1.2331034865516739E-2</v>
+        <v>1.2468365953010077E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="2"/>
-        <v>-4.3956360346290246</v>
+        <v>-4.3845605661274503</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="22" customHeight="1">
@@ -3926,19 +3949,19 @@
       </c>
       <c r="C30" s="10">
         <f t="shared" si="0"/>
-        <v>23.310643589059712</v>
+        <v>23.548325954890156</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="3"/>
-        <v>2.8539250831850516</v>
+        <v>2.1073575332455761</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="1"/>
-        <v>5.3413402542125565E-2</v>
+        <v>5.30652941868325E-2</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="2"/>
-        <v>-2.929693580572251</v>
+        <v>-2.9362321578878832</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="22" customHeight="1">
@@ -3950,19 +3973,19 @@
       </c>
       <c r="C31" s="10">
         <f t="shared" si="0"/>
-        <v>20.271306497143939</v>
+        <v>20.351382408997384</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="3"/>
-        <v>35.259525294135329</v>
+        <v>36.216914677101343</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" si="1"/>
-        <v>3.9310734692701521E-2</v>
+        <v>3.8777807904119221E-2</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="2"/>
-        <v>-3.2362576500078948</v>
+        <v>-3.2499071572191736</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="22" customHeight="1">
@@ -3974,19 +3997,19 @@
       </c>
       <c r="C32" s="10">
         <f t="shared" si="0"/>
-        <v>19.948752048813521</v>
+        <v>20.014889205525826</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="3"/>
-        <v>7.7399990735550244</v>
+        <v>8.112371630865125</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" si="1"/>
-        <v>5.100064956556568E-2</v>
+        <v>5.0214327442153858E-2</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9759169097592015</v>
+        <v>-2.9914548857911245</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="22" customHeight="1">
@@ -3998,19 +4021,19 @@
       </c>
       <c r="C33" s="10">
         <f t="shared" si="0"/>
-        <v>28.302884225224197</v>
+        <v>28.904657351099388</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="3"/>
-        <v>9.2714818463983915E-4</v>
+        <v>0.3264111332763851</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
-        <v>5.4874660424233251E-2</v>
+        <v>5.3941541079111532E-2</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9027035957748186</v>
+        <v>-2.9198543914318908</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="22" customHeight="1">
@@ -4022,19 +4045,19 @@
       </c>
       <c r="C34" s="10">
         <f t="shared" ref="C34:C65" si="4">alpha*(A34-c_)/(alpha/gamma+(A34-c_))</f>
-        <v>30.364699049559029</v>
+        <v>31.155974634597946</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="3"/>
-        <v>313.22035022590552</v>
+        <v>341.85450913300588</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" ref="E34:E65" si="5">NORMDIST(B34,C34,$I$5,FALSE)</f>
-        <v>2.8346752997409764E-3</v>
+        <v>2.3330427932341507E-3</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="2"/>
-        <v>-5.8658278810810263</v>
+        <v>-6.0605819435332053</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="22" customHeight="1">
@@ -4046,19 +4069,19 @@
       </c>
       <c r="C35" s="10">
         <f t="shared" si="4"/>
-        <v>30.364699049559029</v>
+        <v>31.155974634597946</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="3"/>
-        <v>9.8380815435293372E-4</v>
+        <v>0.67673871054639023</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" si="5"/>
-        <v>5.4874631010560913E-2</v>
+        <v>5.3768040025620502E-2</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9027041317905313</v>
+        <v>-2.9230760399013342</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="22" customHeight="1">
@@ -4070,19 +4093,19 @@
       </c>
       <c r="C36" s="10">
         <f t="shared" si="4"/>
-        <v>30.364699049559029</v>
+        <v>31.155974634597946</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="3"/>
-        <v>28.779995892339546</v>
+        <v>37.89602370181332</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" si="5"/>
-        <v>4.1795780733881176E-2</v>
+        <v>3.8183628952263945E-2</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1749598839269817</v>
+        <v>-3.2653484166873743</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="22" customHeight="1">
@@ -4094,19 +4117,19 @@
       </c>
       <c r="C37" s="10">
         <f t="shared" si="4"/>
-        <v>1.2631522318591937</v>
+        <v>1.3877742311444066</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="3"/>
-        <v>1.9698527687129499</v>
+        <v>1.6355658616360669</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" si="5"/>
-        <v>5.3861999782778537E-2</v>
+        <v>5.3296025818164346E-2</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9213300630124568</v>
+        <v>-2.9318935131012482</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="22" customHeight="1">
@@ -4118,19 +4141,19 @@
       </c>
       <c r="C38" s="10">
         <f t="shared" si="4"/>
-        <v>3.2957873772232635</v>
+        <v>3.3348092481892548</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="3"/>
-        <v>4.1702795301353665E-2</v>
+        <v>2.7287984483799207E-2</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" si="5"/>
-        <v>5.4853496795737512E-2</v>
+        <v>5.4090125972521753E-2</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9030893423196318</v>
+        <v>-2.9171036241586079</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="22" customHeight="1">
@@ -4142,19 +4165,19 @@
       </c>
       <c r="C39" s="10">
         <f t="shared" si="4"/>
-        <v>23.186008834521875</v>
+        <v>23.416286942539003</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="3"/>
-        <v>16.155111462298738</v>
+        <v>18.059272489104988</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" si="5"/>
-        <v>4.7097954184913401E-2</v>
+        <v>4.582490262492684E-2</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0555257144675876</v>
+        <v>-3.0829276101920282</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="22" customHeight="1">
@@ -4166,19 +4189,19 @@
       </c>
       <c r="C40" s="10">
         <f t="shared" si="4"/>
-        <v>19.995755378697684</v>
+        <v>20.063890697404027</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="3"/>
-        <v>113.86834771570456</v>
+        <v>112.41885825437402</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="5"/>
-        <v>1.8687240534261542E-2</v>
+        <v>1.9241842468737787E-2</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="2"/>
-        <v>-3.9799143123818537</v>
+        <v>-3.9506680759210946</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="22" customHeight="1">
@@ -4190,19 +4213,19 @@
       </c>
       <c r="C41" s="10">
         <f t="shared" si="4"/>
-        <v>22.970461176423655</v>
+        <v>23.188125356697871</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="3"/>
-        <v>84.570195418776322</v>
+        <v>80.614204054816781</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="5"/>
-        <v>2.4655694764971987E-2</v>
+        <v>2.5779151338904845E-2</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="2"/>
-        <v>-3.702747380227438</v>
+        <v>-3.6581892013727306</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="22" customHeight="1">
@@ -4214,19 +4237,19 @@
       </c>
       <c r="C42" s="10">
         <f t="shared" si="4"/>
-        <v>24.207031365836105</v>
+        <v>24.500360475015977</v>
       </c>
       <c r="D42" s="4">
         <f t="shared" si="3"/>
-        <v>504.43521784631582</v>
+        <v>491.34513018201318</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" si="5"/>
-        <v>4.6440089866026975E-4</v>
+        <v>5.9004421341081784E-4</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>-7.6747623730427765</v>
+        <v>-7.4353130858877821</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="22" customHeight="1">
@@ -4238,19 +4261,19 @@
       </c>
       <c r="C43" s="10">
         <f t="shared" si="4"/>
-        <v>22.970461176423655</v>
+        <v>23.188125356697871</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="3"/>
-        <v>3.4702926729891952</v>
+        <v>2.7067092863848439</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="5"/>
-        <v>5.3102856744291681E-2</v>
+        <v>5.2773618734318066E-2</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9355245528538489</v>
+        <v>-2.9417438583175395</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="22" customHeight="1">
@@ -4262,19 +4285,19 @@
       </c>
       <c r="C44" s="10">
         <f t="shared" si="4"/>
-        <v>26.517926802433134</v>
+        <v>26.974264822846905</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="3"/>
-        <v>26.509522189547877</v>
+        <v>22.018635063883409</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" si="5"/>
-        <v>4.2703230501254595E-2</v>
+        <v>4.4186396176869619E-2</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1534807058422247</v>
+        <v>-3.119338316075956</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="22" customHeight="1">
@@ -4286,19 +4309,19 @@
       </c>
       <c r="C45" s="10">
         <f t="shared" si="4"/>
-        <v>26.080670277537404</v>
+        <v>26.503988575926982</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="3"/>
-        <v>0.56650167556001607</v>
+        <v>0.10846796923102643</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" si="5"/>
-        <v>5.4581839875398781E-2</v>
+        <v>5.4049760626078226E-2</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9080540545706026</v>
+        <v>-2.9178501636564356</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="22" customHeight="1">
@@ -4310,19 +4333,19 @@
       </c>
       <c r="C46" s="10">
         <f t="shared" si="4"/>
-        <v>20.201103458487133</v>
+        <v>20.278100447737913</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="3"/>
-        <v>89.596886848042658</v>
+        <v>88.145175647210777</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" si="5"/>
-        <v>2.3510668522748655E-2</v>
+        <v>2.4054220927069082E-2</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="2"/>
-        <v>-3.7503009811581944</v>
+        <v>-3.7274447915067612</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="22" customHeight="1">
@@ -4334,19 +4357,19 @@
       </c>
       <c r="C47" s="10">
         <f t="shared" si="4"/>
-        <v>23.190064723712116</v>
+        <v>23.420582506301621</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="3"/>
-        <v>58.419555038820555</v>
+        <v>54.948874823658848</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" si="5"/>
-        <v>3.1576042344457107E-2</v>
+        <v>3.2641584957324249E-2</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="2"/>
-        <v>-3.4553565995895186</v>
+        <v>-3.4221681913236166</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="22" customHeight="1">
@@ -4358,19 +4381,19 @@
       </c>
       <c r="C48" s="10">
         <f t="shared" si="4"/>
-        <v>14.927729467007815</v>
+        <v>14.844462359821591</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="3"/>
-        <v>188.75839537617071</v>
+        <v>191.05333190016748</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" si="5"/>
-        <v>9.2014835570887101E-3</v>
+        <v>9.3367337676429091E-3</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" si="2"/>
-        <v>-4.6883905517222324</v>
+        <v>-4.6737987915804657</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="22" customHeight="1">
@@ -4382,19 +4405,19 @@
       </c>
       <c r="C49" s="10">
         <f t="shared" si="4"/>
-        <v>14.510867695537245</v>
+        <v>14.420826337973304</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="3"/>
-        <v>31.988062001829</v>
+        <v>33.014681082839424</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" si="5"/>
-        <v>4.0546375278489193E-2</v>
+        <v>3.993671960699547E-2</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" si="2"/>
-        <v>-3.2053088913559917</v>
+        <v>-3.2204590873922196</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="22" customHeight="1">
@@ -4406,19 +4429,19 @@
       </c>
       <c r="C50" s="10">
         <f t="shared" si="4"/>
-        <v>18.554546417904163</v>
+        <v>18.56651622702044</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="3"/>
-        <v>192.87320398483237</v>
+        <v>193.20581780046689</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" si="5"/>
-        <v>8.8501794651551467E-3</v>
+        <v>9.1537351165153387E-3</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="2"/>
-        <v>-4.7273175416193016</v>
+        <v>-4.6935932735342911</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="22" customHeight="1">
@@ -4430,19 +4453,19 @@
       </c>
       <c r="C51" s="10">
         <f t="shared" si="4"/>
-        <v>26.617420636574153</v>
+        <v>27.081414689954478</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="3"/>
-        <v>1.2486288790417843</v>
+        <v>2.5008724216038183</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" si="5"/>
-        <v>5.4230753310970756E-2</v>
+        <v>5.2873608364130881E-2</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9145071271880156</v>
+        <v>-2.9398509613165542</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="22" customHeight="1">
@@ -4454,19 +4477,19 @@
       </c>
       <c r="C52" s="10">
         <f t="shared" si="4"/>
-        <v>18.800773953101771</v>
+        <v>18.821594527139329</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="3"/>
-        <v>143.21963498768363</v>
+        <v>143.71840645091481</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="5"/>
-        <v>1.4156464373551145E-2</v>
+        <v>1.4429191402037802E-2</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="2"/>
-        <v>-4.257583913027978</v>
+        <v>-4.2385019436612428</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="22" customHeight="1">
@@ -4478,19 +4501,19 @@
       </c>
       <c r="C53" s="10">
         <f t="shared" si="4"/>
-        <v>12.635289874772404</v>
+        <v>12.525260078276716</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="3"/>
-        <v>4.5594628493055493</v>
+        <v>4.10167838466141</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="5"/>
-        <v>5.2558505411254015E-2</v>
+        <v>5.2100947835523354E-2</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9458283410690305</v>
+        <v>-2.9545721377678897</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="22" customHeight="1">
@@ -4502,19 +4525,19 @@
       </c>
       <c r="C54" s="10">
         <f t="shared" si="4"/>
-        <v>11.920771545495111</v>
+        <v>11.807609923320724</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="3"/>
-        <v>60.126142471871034</v>
+        <v>58.384013851407069</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="5"/>
-        <v>3.1070350018323086E-2</v>
+        <v>3.1626557520209514E-2</v>
       </c>
       <c r="F54" s="3">
         <f t="shared" si="2"/>
-        <v>-3.4715012901651585</v>
+        <v>-3.4537580834962833</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="22" customHeight="1">
@@ -4526,19 +4549,19 @@
       </c>
       <c r="C55" s="10">
         <f t="shared" si="4"/>
-        <v>24.097585807359103</v>
+        <v>24.383894824039889</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="3"/>
-        <v>4.9985669998997446</v>
+        <v>3.8003105015161189</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" si="5"/>
-        <v>5.2340629102090155E-2</v>
+        <v>5.2245541198814603E-2</v>
       </c>
       <c r="F55" s="3">
         <f t="shared" si="2"/>
-        <v>-2.9499823624244739</v>
+        <v>-2.9518007276863867</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="22" customHeight="1">
@@ -4550,19 +4573,19 @@
       </c>
       <c r="C56" s="10">
         <f t="shared" si="4"/>
-        <v>22.679194449701935</v>
+        <v>22.880198022981833</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="3"/>
-        <v>74.894119817180325</v>
+        <v>71.455496575110786</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="5"/>
-        <v>2.7019145070083888E-2</v>
+        <v>2.8044442795992493E-2</v>
       </c>
       <c r="F56" s="3">
         <f t="shared" si="2"/>
-        <v>-3.6112095875841206</v>
+        <v>-3.5739647844312823</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="22" customHeight="1">
@@ -4574,19 +4597,19 @@
       </c>
       <c r="C57" s="10">
         <f t="shared" si="4"/>
-        <v>27.803808280088106</v>
+        <v>28.363188293237872</v>
       </c>
       <c r="D57" s="4">
         <f t="shared" si="3"/>
-        <v>204.59893131351706</v>
+        <v>220.91436624024334</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="5"/>
-        <v>7.9209392490626664E-3</v>
+        <v>7.0947235173482682E-3</v>
       </c>
       <c r="F57" s="3">
         <f t="shared" si="2"/>
-        <v>-4.838245488133917</v>
+        <v>-4.9484039377907019</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="22" customHeight="1">
@@ -4598,19 +4621,19 @@
       </c>
       <c r="C58" s="10">
         <f t="shared" si="4"/>
-        <v>23.235278147533577</v>
+        <v>23.468473538312889</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="3"/>
-        <v>79.244621475067206</v>
+        <v>83.450786564634527</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="5"/>
-        <v>2.5929699061462082E-2</v>
+        <v>2.5115384151920165E-2</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" si="2"/>
-        <v>-3.6523662853044621</v>
+        <v>-3.6842747061805965</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="22" customHeight="1">
@@ -4622,19 +4645,19 @@
       </c>
       <c r="C59" s="10">
         <f t="shared" si="4"/>
-        <v>12.178027908305181</v>
+        <v>12.065710519857122</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="3"/>
-        <v>21.671868600296243</v>
+        <v>22.730227291578508</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="5"/>
-        <v>4.4702965188662326E-2</v>
+        <v>4.389818992773039E-2</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="2"/>
-        <v>-3.1077154442458732</v>
+        <v>-3.1258821914656316</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="22" customHeight="1">
@@ -4646,19 +4669,19 @@
       </c>
       <c r="C60" s="10">
         <f t="shared" si="4"/>
-        <v>12.178027908305181</v>
+        <v>12.065710519857122</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="3"/>
-        <v>16.091019010919656</v>
+        <v>15.20254296910225</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="5"/>
-        <v>4.7126519681437648E-2</v>
+        <v>4.7044711009060096E-2</v>
       </c>
       <c r="F60" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0549193858519481</v>
+        <v>-3.0566568314042142</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="22" customHeight="1">
@@ -4670,19 +4693,19 @@
       </c>
       <c r="C61" s="10">
         <f t="shared" si="4"/>
-        <v>19.419367919116898</v>
+        <v>19.4637767666045</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="3"/>
-        <v>60.104376709742866</v>
+        <v>60.794925910552053</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="5"/>
-        <v>3.1076748337786141E-2</v>
+        <v>3.0933081191945117E-2</v>
       </c>
       <c r="F61" s="3">
         <f t="shared" si="2"/>
-        <v>-3.4712953812923422</v>
+        <v>-3.4759290790137762</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="22" customHeight="1">
@@ -4694,19 +4717,19 @@
       </c>
       <c r="C62" s="10">
         <f t="shared" si="4"/>
-        <v>15.593246188412447</v>
+        <v>15.522564269026306</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="3"/>
-        <v>57.356697740440872</v>
+        <v>58.432301465611616</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="5"/>
-        <v>3.189513664901255E-2</v>
+        <v>3.1612516616102468E-2</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" si="2"/>
-        <v>-3.4453017369577648</v>
+        <v>-3.4542021413680826</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="22" customHeight="1">
@@ -4718,19 +4741,19 @@
       </c>
       <c r="C63" s="10">
         <f t="shared" si="4"/>
-        <v>17.336145126555436</v>
+        <v>17.30880802875247</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="3"/>
-        <v>14.672895269256365</v>
+        <v>14.883073270129438</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="5"/>
-        <v>4.7763017809762255E-2</v>
+        <v>4.7183125771083682E-2</v>
       </c>
       <c r="F63" s="3">
         <f t="shared" si="2"/>
-        <v>-3.0415036249224316</v>
+        <v>-3.053718955160643</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="22" customHeight="1">
@@ -4742,19 +4765,19 @@
       </c>
       <c r="C64" s="10">
         <f t="shared" si="4"/>
-        <v>30.382203583998482</v>
+        <v>31.175187685216709</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="3"/>
-        <v>43.795229403642537</v>
+        <v>33.92843850245108</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="5"/>
-        <v>3.6261189161528304E-2</v>
+        <v>3.9602537095682129E-2</v>
       </c>
       <c r="F64" s="3">
         <f t="shared" si="2"/>
-        <v>-3.3170072787842457</v>
+        <v>-3.2288620947011926</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="22" customHeight="1">
@@ -4766,19 +4789,19 @@
       </c>
       <c r="C65" s="10">
         <f t="shared" si="4"/>
-        <v>30.382203583998482</v>
+        <v>31.175187685216709</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="3"/>
-        <v>14.32216082407863</v>
+        <v>8.9489464964570722</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="5"/>
-        <v>4.7921759887436133E-2</v>
+        <v>4.9829499325724891E-2</v>
       </c>
       <c r="F65" s="3">
         <f t="shared" si="2"/>
-        <v>-3.038185600318505</v>
+        <v>-2.9991481143868053</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="22" customHeight="1">
@@ -4790,19 +4813,19 @@
       </c>
       <c r="C66" s="10">
         <f t="shared" ref="C66:C78" si="6">alpha*(A66-c_)/(alpha/gamma+(A66-c_))</f>
-        <v>30.382203583998482</v>
+        <v>31.175187685216709</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="3"/>
-        <v>1.477529997396452</v>
+        <v>4.0341566819571675</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" ref="E66:E78" si="7">NORMDIST(B66,C66,$I$5,FALSE)</f>
-        <v>5.4113446130436005E-2</v>
+        <v>5.213330926343538E-2</v>
       </c>
       <c r="F66" s="3">
         <f t="shared" ref="F66:F78" si="8">LN(E66)</f>
-        <v>-2.9166725818589483</v>
+        <v>-2.9539512012379525</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="22" customHeight="1">
@@ -4814,19 +4837,19 @@
       </c>
       <c r="C67" s="10">
         <f t="shared" si="6"/>
-        <v>4.3769613871895698</v>
+        <v>4.3780438016852212</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" ref="D67:D78" si="9">(C67-B67)^2</f>
-        <v>0.91464729937080402</v>
+        <v>0.91257808927646378</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" si="7"/>
-        <v>5.4402368451429581E-2</v>
+        <v>5.3651554091105717E-2</v>
       </c>
       <c r="F67" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9113475883578763</v>
+        <v>-2.9252448431095806</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="22" customHeight="1">
@@ -4838,19 +4861,19 @@
       </c>
       <c r="C68" s="10">
         <f t="shared" si="6"/>
-        <v>4.3769613871895698</v>
+        <v>4.3780438016852212</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="9"/>
-        <v>2.6342543386736055</v>
+        <v>2.6307419092517299</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="7"/>
-        <v>5.3524518129900278E-2</v>
+        <v>5.2810499467052338E-2</v>
       </c>
       <c r="F68" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9276154472577929</v>
+        <v>-2.9410452544960082</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="22" customHeight="1">
@@ -4862,19 +4885,19 @@
       </c>
       <c r="C69" s="10">
         <f t="shared" si="6"/>
-        <v>5.8746348201716199</v>
+        <v>5.8319670455053734</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="9"/>
-        <v>0.39108160814178222</v>
+        <v>0.44626802829081991</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="7"/>
-        <v>5.4672494306231556E-2</v>
+        <v>5.3882118585004725E-2</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9063945423449895</v>
+        <v>-2.9209566077786158</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="22" customHeight="1">
@@ -4886,19 +4909,19 @@
       </c>
       <c r="C70" s="10">
         <f t="shared" si="6"/>
-        <v>5.8746348201716199</v>
+        <v>5.8319670455053734</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="9"/>
-        <v>3.5142557089998814</v>
+        <v>3.3561032558176866</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="7"/>
-        <v>5.3080775861328311E-2</v>
+        <v>5.2459399463545539E-2</v>
       </c>
       <c r="F70" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9359404527951076</v>
+        <v>-2.9477157521204549</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="22" customHeight="1">
@@ -4910,19 +4933,19 @@
       </c>
       <c r="C71" s="10">
         <f t="shared" si="6"/>
-        <v>5.8746348201716199</v>
+        <v>5.8319670455053734</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="9"/>
-        <v>0.62731444586235807</v>
+        <v>0.69672345756681153</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="7"/>
-        <v>5.455044785829341E-2</v>
+        <v>5.3758159346888559E-2</v>
       </c>
       <c r="F71" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9086293566855512</v>
+        <v>-2.9232598216925147</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="22" customHeight="1">
@@ -4934,19 +4957,19 @@
       </c>
       <c r="C72" s="10">
         <f t="shared" si="6"/>
-        <v>23.725951458750369</v>
+        <v>23.988892261250552</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="9"/>
-        <v>47.508184622827912</v>
+        <v>51.202023570896287</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="7"/>
-        <v>3.5009611262944232E-2</v>
+        <v>3.3785898711244496E-2</v>
       </c>
       <c r="F72" s="3">
         <f t="shared" si="8"/>
-        <v>-3.3521326476777729</v>
+        <v>-3.3877117614365919</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="22" customHeight="1">
@@ -4958,19 +4981,19 @@
       </c>
       <c r="C73" s="10">
         <f t="shared" si="6"/>
-        <v>24.202680500666578</v>
+        <v>24.495729333632561</v>
       </c>
       <c r="D73" s="4">
         <f t="shared" si="9"/>
-        <v>51.878606394682542</v>
+        <v>56.185958243079632</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="7"/>
-        <v>3.3591648682081941E-2</v>
+        <v>3.227234724712285E-2</v>
       </c>
       <c r="F73" s="3">
         <f t="shared" si="8"/>
-        <v>-3.393477794035443</v>
+        <v>-3.4335445378156866</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="22" customHeight="1">
@@ -4982,19 +5005,19 @@
       </c>
       <c r="C74" s="10">
         <f t="shared" si="6"/>
-        <v>23.544630642500312</v>
+        <v>23.796432805521217</v>
       </c>
       <c r="D74" s="4">
         <f t="shared" si="9"/>
-        <v>0.14285676702795155</v>
+        <v>0.39660538964772712</v>
       </c>
       <c r="E74" s="3">
         <f t="shared" si="7"/>
-        <v>5.4801030468893674E-2</v>
+        <v>5.3906732316248825E-2</v>
       </c>
       <c r="F74" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9040462810280716</v>
+        <v>-2.92049990504051</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="22" customHeight="1">
@@ -5006,19 +5029,19 @@
       </c>
       <c r="C75" s="10">
         <f t="shared" si="6"/>
-        <v>29.154357264830104</v>
+        <v>29.831576411926889</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="9"/>
-        <v>6.3116985305565558</v>
+        <v>3.3675562430410233</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="7"/>
-        <v>5.1694448928109031E-2</v>
+        <v>5.2453874581054966E-2</v>
       </c>
       <c r="F75" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9624048740620261</v>
+        <v>-2.9478210749701326</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="22" customHeight="1">
@@ -5030,19 +5053,19 @@
       </c>
       <c r="C76" s="10">
         <f t="shared" si="6"/>
-        <v>29.341505115339512</v>
+        <v>30.035836030012423</v>
       </c>
       <c r="D76" s="4">
         <f t="shared" si="9"/>
-        <v>3.3312146884430671</v>
+        <v>1.2787779287959182</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="7"/>
-        <v>5.3172770589718227E-2</v>
+        <v>5.3471180389193428E-2</v>
       </c>
       <c r="F76" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9342088446850814</v>
+        <v>-2.928612454536839</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="22" customHeight="1">
@@ -5054,19 +5077,19 @@
       </c>
       <c r="C77" s="10">
         <f t="shared" si="6"/>
-        <v>29.392523271086592</v>
+        <v>30.091552179659562</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="9"/>
-        <v>34.721830500297031</v>
+        <v>43.448560137174724</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="7"/>
-        <v>3.9511206454943423E-2</v>
+        <v>3.6282849554445835E-2</v>
       </c>
       <c r="F77" s="3">
         <f t="shared" si="8"/>
-        <v>-3.2311709395923991</v>
+        <v>-3.3164101134224984</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="22" customHeight="1">
@@ -5078,19 +5101,19 @@
       </c>
       <c r="C78" s="10">
         <f t="shared" si="6"/>
-        <v>29.574621330127108</v>
+        <v>30.290534714401588</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="9"/>
-        <v>5.0233718845720015</v>
+        <v>8.7450400081921877</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="7"/>
-        <v>5.2328348310016509E-2</v>
+        <v>4.9923024524470637E-2</v>
       </c>
       <c r="F78" s="3">
         <f t="shared" si="8"/>
-        <v>-2.95021702206162</v>
+        <v>-2.9972729693270095</v>
       </c>
     </row>
   </sheetData>
@@ -5109,9 +5132,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>